<commit_message>
Correction d'un facteur de 500 de la production solaire
</commit_message>
<xml_diff>
--- a/Projet-Groupe1-DKM/data/power_profile.xlsx
+++ b/Projet-Groupe1-DKM/data/power_profile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\karim\git\rhtlab_DKM\Projet-Groupe1-DKM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACC1199-B4EA-4AEF-BF5F-73BBBB3F1846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E1E1FE-8558-4746-8998-80DC7F224422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="load" sheetId="5" r:id="rId1"/>
@@ -431,7 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB91AA0C-6E10-4C2C-B831-A2E20673E5F8}">
   <dimension ref="A1:AV98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AB3" sqref="AB3:AY98"/>
     </sheetView>
   </sheetViews>
@@ -10229,6 +10229,14 @@
     <protectedRange sqref="T3:W98" name="Plage1_13"/>
   </protectedRanges>
   <mergeCells count="20">
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -10241,14 +10249,6 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10258,8 +10258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0724F9-1790-4ECA-B4EA-D773CFA5B42B}">
   <dimension ref="A1:AM98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10508,13 +10508,13 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="B4">
-        <v>2.450999683732439</v>
+        <v>4.9019993674648777E-3</v>
       </c>
       <c r="C4" s="7">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1.8382497627993291</v>
+        <v>3.6764995255986581E-3</v>
       </c>
       <c r="E4" s="7">
         <v>0</v>
@@ -10545,13 +10545,13 @@
         <v>8.3333333333333301E-2</v>
       </c>
       <c r="B5">
-        <v>4.8563418808264371</v>
+        <v>9.7126837616528742E-3</v>
       </c>
       <c r="C5" s="7">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>3.6422564106198281</v>
+        <v>7.2845128212396561E-3</v>
       </c>
       <c r="E5" s="7">
         <v>0</v>
@@ -10582,13 +10582,13 @@
         <v>0.125</v>
       </c>
       <c r="B6">
-        <v>7.1712196172323459</v>
+        <v>1.4342439234464693E-2</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>5.3784147129242594</v>
+        <v>1.0756829425848519E-2</v>
       </c>
       <c r="E6" s="7">
         <v>0</v>
@@ -10619,13 +10619,13 @@
         <v>0.16666666666666699</v>
       </c>
       <c r="B7">
-        <v>9.3525111006378019</v>
+        <v>1.8705022201275602E-2</v>
       </c>
       <c r="C7" s="7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>7.0143833254783514</v>
+        <v>1.4028766650956703E-2</v>
       </c>
       <c r="E7" s="7">
         <v>0</v>
@@ -10656,13 +10656,13 @@
         <v>0.20833333333333301</v>
       </c>
       <c r="B8">
-        <v>11.35958299786895</v>
+        <v>2.2719165995737898E-2</v>
       </c>
       <c r="C8" s="7">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>8.519687248401711</v>
+        <v>1.7039374496803421E-2</v>
       </c>
       <c r="E8" s="7">
         <v>0</v>
@@ -10693,13 +10693,13 @@
         <v>0.25</v>
       </c>
       <c r="B9">
-        <v>13.155047357006231</v>
+        <v>2.6310094714012459E-2</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>9.866285517754676</v>
+        <v>1.9732571035509353E-2</v>
       </c>
       <c r="E9" s="7">
         <v>0</v>
@@ -10730,13 +10730,13 @@
         <v>0.29166666666666702</v>
       </c>
       <c r="B10">
-        <v>14.705458074187961</v>
+        <v>2.9410916148375921E-2</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>11.029093555640969</v>
+        <v>2.2058187111281938E-2</v>
       </c>
       <c r="E10" s="7">
         <v>0</v>
@@ -10767,13 +10767,13 @@
         <v>0.33333333333333298</v>
       </c>
       <c r="B11">
-        <v>15.98193393124275</v>
+        <v>3.19638678624855E-2</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>11.986450448432061</v>
+        <v>2.3972900896864123E-2</v>
       </c>
       <c r="E11" s="7">
         <v>0</v>
@@ -10804,13 +10804,13 @@
         <v>0.375</v>
       </c>
       <c r="B12">
-        <v>16.960696598138771</v>
+        <v>3.3921393196277544E-2</v>
       </c>
       <c r="C12" s="7">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>12.720522448604081</v>
+        <v>2.5441044897208161E-2</v>
       </c>
       <c r="E12" s="7">
         <v>0</v>
@@ -10841,13 +10841,13 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="B13">
-        <v>17.623513578281809</v>
+        <v>3.5247027156563616E-2</v>
       </c>
       <c r="C13" s="7">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>13.21763518371136</v>
+        <v>2.6435270367422721E-2</v>
       </c>
       <c r="E13" s="7">
         <v>0</v>
@@ -10878,13 +10878,13 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="B14">
-        <v>17.958037845429711</v>
+        <v>3.5916075690859424E-2</v>
       </c>
       <c r="C14" s="7">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>13.468528384072281</v>
+        <v>2.6937056768144563E-2</v>
       </c>
       <c r="E14" s="7">
         <v>0</v>
@@ -10915,13 +10915,13 @@
         <v>0.5</v>
       </c>
       <c r="B15">
-        <v>17.9580378454297</v>
+        <v>3.5916075690859403E-2</v>
       </c>
       <c r="C15" s="7">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>13.468528384072281</v>
+        <v>2.6937056768144563E-2</v>
       </c>
       <c r="E15" s="7">
         <v>0</v>
@@ -10952,13 +10952,13 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="B16">
-        <v>17.62351357828182</v>
+        <v>3.5247027156563637E-2</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>13.21763518371136</v>
+        <v>2.6435270367422721E-2</v>
       </c>
       <c r="E16" s="7">
         <v>0</v>
@@ -10989,13 +10989,13 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="B17">
-        <v>16.960696598138771</v>
+        <v>3.3921393196277544E-2</v>
       </c>
       <c r="C17" s="7">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>12.720522448604081</v>
+        <v>2.5441044897208161E-2</v>
       </c>
       <c r="E17" s="7">
         <v>0</v>
@@ -11026,13 +11026,13 @@
         <v>0.625</v>
       </c>
       <c r="B18">
-        <v>15.981933931242761</v>
+        <v>3.196386786248552E-2</v>
       </c>
       <c r="C18" s="7">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>11.986450448432061</v>
+        <v>2.3972900896864123E-2</v>
       </c>
       <c r="E18" s="7">
         <v>0</v>
@@ -11063,13 +11063,13 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B19">
-        <v>14.705458074187961</v>
+        <v>2.9410916148375921E-2</v>
       </c>
       <c r="C19" s="7">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>11.029093555640969</v>
+        <v>2.2058187111281938E-2</v>
       </c>
       <c r="E19" s="7">
         <v>0</v>
@@ -11100,13 +11100,13 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B20">
-        <v>13.155047357006239</v>
+        <v>2.631009471401248E-2</v>
       </c>
       <c r="C20" s="7">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>9.8662855177546795</v>
+        <v>1.973257103550936E-2</v>
       </c>
       <c r="E20" s="7">
         <v>0</v>
@@ -11137,13 +11137,13 @@
         <v>0.75</v>
       </c>
       <c r="B21">
-        <v>11.35958299786895</v>
+        <v>2.2719165995737898E-2</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>8.5196872484017145</v>
+        <v>1.7039374496803428E-2</v>
       </c>
       <c r="E21" s="7">
         <v>0</v>
@@ -11174,13 +11174,13 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="B22">
-        <v>9.352511100637809</v>
+        <v>1.8705022201275619E-2</v>
       </c>
       <c r="C22" s="7">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>7.0143833254783559</v>
+        <v>1.4028766650956712E-2</v>
       </c>
       <c r="E22" s="7">
         <v>0</v>
@@ -11211,13 +11211,13 @@
         <v>0.83333333333333304</v>
       </c>
       <c r="B23">
-        <v>7.171219617232353</v>
+        <v>1.4342439234464707E-2</v>
       </c>
       <c r="C23" s="7">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>5.3784147129242648</v>
+        <v>1.0756829425848529E-2</v>
       </c>
       <c r="E23" s="7">
         <v>0</v>
@@ -11248,13 +11248,13 @@
         <v>0.875</v>
       </c>
       <c r="B24">
-        <v>4.8563418808264371</v>
+        <v>9.7126837616528742E-3</v>
       </c>
       <c r="C24" s="7">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>3.6422564106198281</v>
+        <v>7.2845128212396561E-3</v>
       </c>
       <c r="E24" s="7">
         <v>0</v>
@@ -11285,13 +11285,13 @@
         <v>0.91666666666666696</v>
       </c>
       <c r="B25">
-        <v>2.4509996837324399</v>
+        <v>4.9019993674648795E-3</v>
       </c>
       <c r="C25" s="7">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1.8382497627993299</v>
+        <v>3.6764995255986598E-3</v>
       </c>
       <c r="E25" s="7">
         <v>0</v>
@@ -11322,13 +11322,13 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="B26">
-        <v>2.2043642384652358E-15</v>
+        <v>4.4087284769304718E-18</v>
       </c>
       <c r="C26" s="7">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>1.6532731788489271E-15</v>
+        <v>3.306546357697854E-18</v>
       </c>
       <c r="E26" s="7">
         <v>0</v>
@@ -11572,6 +11572,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -11584,14 +11592,6 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Correction de la pruction solaire d'un facteur de 2
</commit_message>
<xml_diff>
--- a/Projet-Groupe1-DKM/data/power_profile.xlsx
+++ b/Projet-Groupe1-DKM/data/power_profile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\karim\git\rhtlab_DKM\Projet-Groupe1-DKM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E1E1FE-8558-4746-8998-80DC7F224422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845FCEFC-37FF-4F06-A045-7E405552905E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
@@ -10229,14 +10229,6 @@
     <protectedRange sqref="T3:W98" name="Plage1_13"/>
   </protectedRanges>
   <mergeCells count="20">
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -10249,6 +10241,14 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10259,7 +10259,7 @@
   <dimension ref="A1:AM98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:J26"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10508,13 +10508,13 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="B4">
-        <v>4.9019993674648777E-3</v>
+        <v>2.4509996837324389E-3</v>
       </c>
       <c r="C4" s="7">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>3.6764995255986581E-3</v>
+        <v>1.838249762799329E-3</v>
       </c>
       <c r="E4" s="7">
         <v>0</v>
@@ -10545,13 +10545,13 @@
         <v>8.3333333333333301E-2</v>
       </c>
       <c r="B5">
-        <v>9.7126837616528742E-3</v>
+        <v>4.8563418808264371E-3</v>
       </c>
       <c r="C5" s="7">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>7.2845128212396561E-3</v>
+        <v>3.642256410619828E-3</v>
       </c>
       <c r="E5" s="7">
         <v>0</v>
@@ -10582,13 +10582,13 @@
         <v>0.125</v>
       </c>
       <c r="B6">
-        <v>1.4342439234464693E-2</v>
+        <v>7.1712196172323463E-3</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1.0756829425848519E-2</v>
+        <v>5.3784147129242593E-3</v>
       </c>
       <c r="E6" s="7">
         <v>0</v>
@@ -10619,13 +10619,13 @@
         <v>0.16666666666666699</v>
       </c>
       <c r="B7">
-        <v>1.8705022201275602E-2</v>
+        <v>9.352511100637801E-3</v>
       </c>
       <c r="C7" s="7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1.4028766650956703E-2</v>
+        <v>7.0143833254783516E-3</v>
       </c>
       <c r="E7" s="7">
         <v>0</v>
@@ -10656,13 +10656,13 @@
         <v>0.20833333333333301</v>
       </c>
       <c r="B8">
-        <v>2.2719165995737898E-2</v>
+        <v>1.1359582997868949E-2</v>
       </c>
       <c r="C8" s="7">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1.7039374496803421E-2</v>
+        <v>8.5196872484017104E-3</v>
       </c>
       <c r="E8" s="7">
         <v>0</v>
@@ -10693,13 +10693,13 @@
         <v>0.25</v>
       </c>
       <c r="B9">
-        <v>2.6310094714012459E-2</v>
+        <v>1.315504735700623E-2</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1.9732571035509353E-2</v>
+        <v>9.8662855177546766E-3</v>
       </c>
       <c r="E9" s="7">
         <v>0</v>
@@ -10730,13 +10730,13 @@
         <v>0.29166666666666702</v>
       </c>
       <c r="B10">
-        <v>2.9410916148375921E-2</v>
+        <v>1.4705458074187961E-2</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>2.2058187111281938E-2</v>
+        <v>1.1029093555640969E-2</v>
       </c>
       <c r="E10" s="7">
         <v>0</v>
@@ -10767,13 +10767,13 @@
         <v>0.33333333333333298</v>
       </c>
       <c r="B11">
-        <v>3.19638678624855E-2</v>
+        <v>1.598193393124275E-2</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>2.3972900896864123E-2</v>
+        <v>1.1986450448432062E-2</v>
       </c>
       <c r="E11" s="7">
         <v>0</v>
@@ -10804,13 +10804,13 @@
         <v>0.375</v>
       </c>
       <c r="B12">
-        <v>3.3921393196277544E-2</v>
+        <v>1.6960696598138772E-2</v>
       </c>
       <c r="C12" s="7">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>2.5441044897208161E-2</v>
+        <v>1.2720522448604081E-2</v>
       </c>
       <c r="E12" s="7">
         <v>0</v>
@@ -10841,13 +10841,13 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="B13">
-        <v>3.5247027156563616E-2</v>
+        <v>1.7623513578281808E-2</v>
       </c>
       <c r="C13" s="7">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>2.6435270367422721E-2</v>
+        <v>1.3217635183711361E-2</v>
       </c>
       <c r="E13" s="7">
         <v>0</v>
@@ -10878,13 +10878,13 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="B14">
-        <v>3.5916075690859424E-2</v>
+        <v>1.7958037845429712E-2</v>
       </c>
       <c r="C14" s="7">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>2.6937056768144563E-2</v>
+        <v>1.3468528384072281E-2</v>
       </c>
       <c r="E14" s="7">
         <v>0</v>
@@ -10915,13 +10915,13 @@
         <v>0.5</v>
       </c>
       <c r="B15">
-        <v>3.5916075690859403E-2</v>
+        <v>1.7958037845429702E-2</v>
       </c>
       <c r="C15" s="7">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>2.6937056768144563E-2</v>
+        <v>1.3468528384072281E-2</v>
       </c>
       <c r="E15" s="7">
         <v>0</v>
@@ -10952,13 +10952,13 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="B16">
-        <v>3.5247027156563637E-2</v>
+        <v>1.7623513578281819E-2</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>2.6435270367422721E-2</v>
+        <v>1.3217635183711361E-2</v>
       </c>
       <c r="E16" s="7">
         <v>0</v>
@@ -10989,13 +10989,13 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="B17">
-        <v>3.3921393196277544E-2</v>
+        <v>1.6960696598138772E-2</v>
       </c>
       <c r="C17" s="7">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>2.5441044897208161E-2</v>
+        <v>1.2720522448604081E-2</v>
       </c>
       <c r="E17" s="7">
         <v>0</v>
@@ -11026,13 +11026,13 @@
         <v>0.625</v>
       </c>
       <c r="B18">
-        <v>3.196386786248552E-2</v>
+        <v>1.598193393124276E-2</v>
       </c>
       <c r="C18" s="7">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>2.3972900896864123E-2</v>
+        <v>1.1986450448432062E-2</v>
       </c>
       <c r="E18" s="7">
         <v>0</v>
@@ -11063,13 +11063,13 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B19">
-        <v>2.9410916148375921E-2</v>
+        <v>1.4705458074187961E-2</v>
       </c>
       <c r="C19" s="7">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>2.2058187111281938E-2</v>
+        <v>1.1029093555640969E-2</v>
       </c>
       <c r="E19" s="7">
         <v>0</v>
@@ -11100,13 +11100,13 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B20">
-        <v>2.631009471401248E-2</v>
+        <v>1.315504735700624E-2</v>
       </c>
       <c r="C20" s="7">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1.973257103550936E-2</v>
+        <v>9.8662855177546801E-3</v>
       </c>
       <c r="E20" s="7">
         <v>0</v>
@@ -11137,13 +11137,13 @@
         <v>0.75</v>
       </c>
       <c r="B21">
-        <v>2.2719165995737898E-2</v>
+        <v>1.1359582997868949E-2</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>1.7039374496803428E-2</v>
+        <v>8.5196872484017139E-3</v>
       </c>
       <c r="E21" s="7">
         <v>0</v>
@@ -11174,13 +11174,13 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="B22">
-        <v>1.8705022201275619E-2</v>
+        <v>9.3525111006378097E-3</v>
       </c>
       <c r="C22" s="7">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>1.4028766650956712E-2</v>
+        <v>7.014383325478356E-3</v>
       </c>
       <c r="E22" s="7">
         <v>0</v>
@@ -11211,13 +11211,13 @@
         <v>0.83333333333333304</v>
       </c>
       <c r="B23">
-        <v>1.4342439234464707E-2</v>
+        <v>7.1712196172323533E-3</v>
       </c>
       <c r="C23" s="7">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>1.0756829425848529E-2</v>
+        <v>5.3784147129242645E-3</v>
       </c>
       <c r="E23" s="7">
         <v>0</v>
@@ -11248,13 +11248,13 @@
         <v>0.875</v>
       </c>
       <c r="B24">
-        <v>9.7126837616528742E-3</v>
+        <v>4.8563418808264371E-3</v>
       </c>
       <c r="C24" s="7">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>7.2845128212396561E-3</v>
+        <v>3.642256410619828E-3</v>
       </c>
       <c r="E24" s="7">
         <v>0</v>
@@ -11285,13 +11285,13 @@
         <v>0.91666666666666696</v>
       </c>
       <c r="B25">
-        <v>4.9019993674648795E-3</v>
+        <v>2.4509996837324397E-3</v>
       </c>
       <c r="C25" s="7">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>3.6764995255986598E-3</v>
+        <v>1.8382497627993299E-3</v>
       </c>
       <c r="E25" s="7">
         <v>0</v>
@@ -11322,13 +11322,13 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="B26">
-        <v>4.4087284769304718E-18</v>
+        <v>2.2043642384652359E-18</v>
       </c>
       <c r="C26" s="7">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>3.306546357697854E-18</v>
+        <v>1.653273178848927E-18</v>
       </c>
       <c r="E26" s="7">
         <v>0</v>
@@ -11572,14 +11572,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -11592,6 +11584,14 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Changement de transfo et ligne
</commit_message>
<xml_diff>
--- a/Projet-Groupe1-DKM/data/power_profile.xlsx
+++ b/Projet-Groupe1-DKM/data/power_profile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\karim\git\rhtlab_DKM\Projet-Groupe1-DKM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845FCEFC-37FF-4F06-A045-7E405552905E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A65241E-E4B9-480A-9797-1DA246EDF9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="4968" yWindow="612" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="load" sheetId="5" r:id="rId1"/>
@@ -10229,6 +10229,14 @@
     <protectedRange sqref="T3:W98" name="Plage1_13"/>
   </protectedRanges>
   <mergeCells count="20">
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -10241,14 +10249,6 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10259,7 +10259,7 @@
   <dimension ref="A1:AM98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10508,13 +10508,13 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="B4">
-        <v>2.4509996837324389E-3</v>
+        <v>2.450999683732439E-2</v>
       </c>
       <c r="C4" s="7">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1.838249762799329E-3</v>
+        <v>1.838249762799329E-2</v>
       </c>
       <c r="E4" s="7">
         <v>0</v>
@@ -10545,13 +10545,13 @@
         <v>8.3333333333333301E-2</v>
       </c>
       <c r="B5">
-        <v>4.8563418808264371E-3</v>
+        <v>4.8563418808264369E-2</v>
       </c>
       <c r="C5" s="7">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>3.642256410619828E-3</v>
+        <v>3.6422564106198277E-2</v>
       </c>
       <c r="E5" s="7">
         <v>0</v>
@@ -10582,13 +10582,13 @@
         <v>0.125</v>
       </c>
       <c r="B6">
-        <v>7.1712196172323463E-3</v>
+        <v>7.1712196172323467E-2</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>5.3784147129242593E-3</v>
+        <v>5.3784147129242593E-2</v>
       </c>
       <c r="E6" s="7">
         <v>0</v>
@@ -10619,13 +10619,13 @@
         <v>0.16666666666666699</v>
       </c>
       <c r="B7">
-        <v>9.352511100637801E-3</v>
+        <v>9.3525111006378003E-2</v>
       </c>
       <c r="C7" s="7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>7.0143833254783516E-3</v>
+        <v>7.0143833254783516E-2</v>
       </c>
       <c r="E7" s="7">
         <v>0</v>
@@ -10656,13 +10656,13 @@
         <v>0.20833333333333301</v>
       </c>
       <c r="B8">
-        <v>1.1359582997868949E-2</v>
+        <v>0.11359582997868949</v>
       </c>
       <c r="C8" s="7">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>8.5196872484017104E-3</v>
+        <v>8.5196872484017111E-2</v>
       </c>
       <c r="E8" s="7">
         <v>0</v>
@@ -10693,13 +10693,13 @@
         <v>0.25</v>
       </c>
       <c r="B9">
-        <v>1.315504735700623E-2</v>
+        <v>0.1315504735700623</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>9.8662855177546766E-3</v>
+        <v>9.8662855177546763E-2</v>
       </c>
       <c r="E9" s="7">
         <v>0</v>
@@ -10730,13 +10730,13 @@
         <v>0.29166666666666702</v>
       </c>
       <c r="B10">
-        <v>1.4705458074187961E-2</v>
+        <v>0.1470545807418796</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1.1029093555640969E-2</v>
+        <v>0.11029093555640969</v>
       </c>
       <c r="E10" s="7">
         <v>0</v>
@@ -10767,13 +10767,13 @@
         <v>0.33333333333333298</v>
       </c>
       <c r="B11">
-        <v>1.598193393124275E-2</v>
+        <v>0.15981933931242751</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1.1986450448432062E-2</v>
+        <v>0.11986450448432062</v>
       </c>
       <c r="E11" s="7">
         <v>0</v>
@@ -10804,13 +10804,13 @@
         <v>0.375</v>
       </c>
       <c r="B12">
-        <v>1.6960696598138772E-2</v>
+        <v>0.16960696598138772</v>
       </c>
       <c r="C12" s="7">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1.2720522448604081E-2</v>
+        <v>0.1272052244860408</v>
       </c>
       <c r="E12" s="7">
         <v>0</v>
@@ -10841,13 +10841,13 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="B13">
-        <v>1.7623513578281808E-2</v>
+        <v>0.17623513578281808</v>
       </c>
       <c r="C13" s="7">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>1.3217635183711361E-2</v>
+        <v>0.1321763518371136</v>
       </c>
       <c r="E13" s="7">
         <v>0</v>
@@ -10878,13 +10878,13 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="B14">
-        <v>1.7958037845429712E-2</v>
+        <v>0.17958037845429711</v>
       </c>
       <c r="C14" s="7">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1.3468528384072281E-2</v>
+        <v>0.13468528384072281</v>
       </c>
       <c r="E14" s="7">
         <v>0</v>
@@ -10915,13 +10915,13 @@
         <v>0.5</v>
       </c>
       <c r="B15">
-        <v>1.7958037845429702E-2</v>
+        <v>0.17958037845429703</v>
       </c>
       <c r="C15" s="7">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>1.3468528384072281E-2</v>
+        <v>0.13468528384072281</v>
       </c>
       <c r="E15" s="7">
         <v>0</v>
@@ -10952,13 +10952,13 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="B16">
-        <v>1.7623513578281819E-2</v>
+        <v>0.17623513578281819</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>1.3217635183711361E-2</v>
+        <v>0.1321763518371136</v>
       </c>
       <c r="E16" s="7">
         <v>0</v>
@@ -10989,13 +10989,13 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="B17">
-        <v>1.6960696598138772E-2</v>
+        <v>0.16960696598138772</v>
       </c>
       <c r="C17" s="7">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1.2720522448604081E-2</v>
+        <v>0.1272052244860408</v>
       </c>
       <c r="E17" s="7">
         <v>0</v>
@@ -11026,13 +11026,13 @@
         <v>0.625</v>
       </c>
       <c r="B18">
-        <v>1.598193393124276E-2</v>
+        <v>0.15981933931242759</v>
       </c>
       <c r="C18" s="7">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>1.1986450448432062E-2</v>
+        <v>0.11986450448432062</v>
       </c>
       <c r="E18" s="7">
         <v>0</v>
@@ -11063,13 +11063,13 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B19">
-        <v>1.4705458074187961E-2</v>
+        <v>0.1470545807418796</v>
       </c>
       <c r="C19" s="7">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>1.1029093555640969E-2</v>
+        <v>0.11029093555640969</v>
       </c>
       <c r="E19" s="7">
         <v>0</v>
@@ -11100,13 +11100,13 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B20">
-        <v>1.315504735700624E-2</v>
+        <v>0.13155047357006239</v>
       </c>
       <c r="C20" s="7">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>9.8662855177546801E-3</v>
+        <v>9.8662855177546804E-2</v>
       </c>
       <c r="E20" s="7">
         <v>0</v>
@@ -11137,13 +11137,13 @@
         <v>0.75</v>
       </c>
       <c r="B21">
-        <v>1.1359582997868949E-2</v>
+        <v>0.11359582997868949</v>
       </c>
       <c r="C21" s="7">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>8.5196872484017139E-3</v>
+        <v>8.5196872484017139E-2</v>
       </c>
       <c r="E21" s="7">
         <v>0</v>
@@ -11174,13 +11174,13 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="B22">
-        <v>9.3525111006378097E-3</v>
+        <v>9.35251110063781E-2</v>
       </c>
       <c r="C22" s="7">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>7.014383325478356E-3</v>
+        <v>7.0143833254783558E-2</v>
       </c>
       <c r="E22" s="7">
         <v>0</v>
@@ -11211,13 +11211,13 @@
         <v>0.83333333333333304</v>
       </c>
       <c r="B23">
-        <v>7.1712196172323533E-3</v>
+        <v>7.1712196172323536E-2</v>
       </c>
       <c r="C23" s="7">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>5.3784147129242645E-3</v>
+        <v>5.3784147129242649E-2</v>
       </c>
       <c r="E23" s="7">
         <v>0</v>
@@ -11248,13 +11248,13 @@
         <v>0.875</v>
       </c>
       <c r="B24">
-        <v>4.8563418808264371E-3</v>
+        <v>4.8563418808264369E-2</v>
       </c>
       <c r="C24" s="7">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>3.642256410619828E-3</v>
+        <v>3.6422564106198277E-2</v>
       </c>
       <c r="E24" s="7">
         <v>0</v>
@@ -11285,13 +11285,13 @@
         <v>0.91666666666666696</v>
       </c>
       <c r="B25">
-        <v>2.4509996837324397E-3</v>
+        <v>2.4509996837324396E-2</v>
       </c>
       <c r="C25" s="7">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1.8382497627993299E-3</v>
+        <v>1.8382497627993301E-2</v>
       </c>
       <c r="E25" s="7">
         <v>0</v>
@@ -11322,13 +11322,13 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="B26">
-        <v>2.2043642384652359E-18</v>
+        <v>2.2043642384652358E-17</v>
       </c>
       <c r="C26" s="7">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>1.653273178848927E-18</v>
+        <v>1.6532731788489269E-17</v>
       </c>
       <c r="E26" s="7">
         <v>0</v>
@@ -11572,6 +11572,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -11584,14 +11592,6 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:U1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>